<commit_message>
paper: projects description and steps for collecting data part
</commit_message>
<xml_diff>
--- a/data/4.Apache commons collections 132K/BMI/Metric 5 (BMI) - Collection.xlsx
+++ b/data/4.Apache commons collections 132K/BMI/Metric 5 (BMI) - Collection.xlsx
@@ -3,23 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B8210-29AC-4017-BC19-A41E4C64CA01}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4BA33F-697B-423C-AC44-93523EED4F32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5472" yWindow="1848" windowWidth="13860" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -64,10 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.1~4.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3.2~4.0（3.2，3.2.1）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -77,6 +67,10 @@
   </si>
   <si>
     <t>https://issues.apache.org/jira/secure/ConfigureReport.jspa?projectOrFilterId=project-12310465&amp;dateField=created&amp;periodName=monthly&amp;daysprevious=7200&amp;cumulative=true&amp;selectedProjectId=12310465&amp;reportKey=com.atlassian.jira.jira-core-reports-plugin%3Atimesince-report&amp;atl_token=A5KQ-2QAV-T4JA-FDED%7C2e411ca6e9b41de8c75e4366f0363a384cbb1fdf%7Clout&amp;Next=Next</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1~4.4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -84,7 +78,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,15 +414,15 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -454,7 +448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>42979</v>
       </c>
@@ -481,10 +475,10 @@
         <v>40.317460317460309</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43009</v>
       </c>
@@ -499,7 +493,7 @@
         <v>14.285714285714285</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43040</v>
       </c>
@@ -514,7 +508,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>41699</v>
       </c>
@@ -544,7 +538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>41730</v>
       </c>
@@ -559,7 +553,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>41760</v>
       </c>
@@ -574,7 +568,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42339</v>
       </c>
@@ -601,10 +595,10 @@
         <v>41.666666666666664</v>
       </c>
       <c r="H8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42461</v>
       </c>
@@ -619,7 +613,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>42979</v>
       </c>
@@ -634,9 +628,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -651,9 +645,9 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -668,10 +662,10 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
   </sheetData>

</xml_diff>